<commit_message>
Made tests for checking if timepoints are formatted correctly
</commit_message>
<xml_diff>
--- a/test_files/perturbation_tests/to_be_reformatted/seaver_post_L-curve/4-genes_6-edges_artificial-data_Sigmoidal_estimation_fixb-1_fixP-1_no-graph_test1.xlsx
+++ b/test_files/perturbation_tests/to_be_reformatted/seaver_post_L-curve/4-genes_6-edges_artificial-data_Sigmoidal_estimation_fixb-1_fixP-1_no-graph_test1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView xWindow="11475" yWindow="-135" windowWidth="6615" windowHeight="12225" tabRatio="644" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="11475" yWindow="-135" windowWidth="6615" windowHeight="12225" tabRatio="644" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="13" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="31">
   <si>
     <t>CIN5</t>
   </si>
@@ -107,13 +107,16 @@
     <t>production_rate</t>
   </si>
   <si>
-    <t>Model</t>
-  </si>
-  <si>
     <t>Sigmoid</t>
   </si>
   <si>
     <t>targets/regulators</t>
+  </si>
+  <si>
+    <t>production_function</t>
+  </si>
+  <si>
+    <t>L_curve</t>
   </si>
 </sst>
 </file>
@@ -1439,7 +1442,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>10</v>
@@ -1534,7 +1537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -1561,7 +1564,7 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
@@ -1683,10 +1686,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V17"/>
+  <dimension ref="A1:V18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1764,39 +1767,39 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>27</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="8">
-        <v>1</v>
+        <v>30</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>15</v>
-      </c>
-      <c r="B11" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>16</v>
       </c>
       <c r="B12" s="8">
         <v>1</v>
@@ -1804,119 +1807,127 @@
     </row>
     <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B14" s="8">
         <v>0.4</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <v>0.8</v>
       </c>
-      <c r="D13">
+      <c r="D14">
         <v>1.2</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <v>1.6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="7">
-        <v>3</v>
-      </c>
-      <c r="C15">
-        <v>4</v>
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B16" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="7">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>22</v>
       </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
         <v>0.1</v>
       </c>
-      <c r="D17">
+      <c r="D18">
         <v>0.2</v>
       </c>
-      <c r="E17">
+      <c r="E18">
         <v>0.30000000000000004</v>
       </c>
-      <c r="F17">
+      <c r="F18">
         <v>0.4</v>
       </c>
-      <c r="G17">
+      <c r="G18">
         <v>0.5</v>
       </c>
-      <c r="H17">
+      <c r="H18">
         <v>0.60000000000000009</v>
       </c>
-      <c r="I17">
+      <c r="I18">
         <v>0.70000000000000007</v>
       </c>
-      <c r="J17">
+      <c r="J18">
         <v>0.8</v>
       </c>
-      <c r="K17">
+      <c r="K18">
         <v>0.9</v>
       </c>
-      <c r="L17">
-        <v>1</v>
-      </c>
-      <c r="M17">
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N17">
+      <c r="N18">
         <v>1.2000000000000002</v>
       </c>
-      <c r="O17">
+      <c r="O18">
         <v>1.3</v>
       </c>
-      <c r="P17">
+      <c r="P18">
         <v>1.4000000000000001</v>
       </c>
-      <c r="Q17">
+      <c r="Q18">
         <v>1.5</v>
       </c>
-      <c r="R17">
+      <c r="R18">
         <v>1.6</v>
       </c>
-      <c r="S17">
+      <c r="S18">
         <v>1.7000000000000002</v>
       </c>
-      <c r="T17">
+      <c r="T18">
         <v>1.8</v>
       </c>
-      <c r="U17">
+      <c r="U18">
         <v>1.9000000000000001</v>
       </c>
-      <c r="V17">
+      <c r="V18">
         <v>2</v>
       </c>
     </row>

</xml_diff>